<commit_message>
updates to prepping heat model output data to summarize rasteration data and calculate added heat from vehicles and pavement across metro
</commit_message>
<xml_diff>
--- a/data/drivecycles/NREL_D3_summary.xlsx
+++ b/data/drivecycles/NREL_D3_summary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="24">
   <si>
     <t>2013 Dodge Ram 1500 HFE</t>
   </si>
@@ -409,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,7 +795,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
-        <v>0.41</v>
+        <v>0.42</v>
       </c>
       <c r="D29" s="1">
         <v>0.12</v>
@@ -811,7 +811,7 @@
       </c>
       <c r="H29" s="1">
         <f>SUM(C29:G29)</f>
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -822,6 +822,38 @@
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>24.9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <f>AVERAGE(C2,C14,C18,C22)</f>
+        <v>23.974999999999998</v>
+      </c>
+      <c r="C35">
+        <f>AVERAGE(C3,C15,C19,C23)</f>
+        <v>40.575000000000003</v>
+      </c>
+      <c r="D35">
+        <f>AVERAGE(C4,C16,C20,C24)</f>
+        <v>26.224999999999998</v>
+      </c>
+      <c r="E35">
+        <f>AVERAGE(C5,C17,C21,C25)</f>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>